<commit_message>
stage changes for rebase'
</commit_message>
<xml_diff>
--- a/template_loadgen.xlsx
+++ b/template_loadgen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBC4C23C-60E2-064C-9862-79C4C8B28F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF38E7E-B781-6047-8298-7D6A26799A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" activeTab="6" xr2:uid="{5A3F0FCA-A9DB-A84C-AEE3-F88E9CDDE907}"/>
+    <workbookView xWindow="1500" yWindow="1300" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{5A3F0FCA-A9DB-A84C-AEE3-F88E9CDDE907}"/>
   </bookViews>
   <sheets>
     <sheet name="load" sheetId="1" r:id="rId1"/>
@@ -718,7 +718,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O50" sqref="O50"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -890,7 +890,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476D1716-E415-9148-A59A-7D3D790AE6BA}">
   <dimension ref="B1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1283,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F287D5-1D76-CB40-9998-8C337CC7B8B4}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
implemented scenarios code, adjusted everything, added conda environment
</commit_message>
<xml_diff>
--- a/template_loadgen.xlsx
+++ b/template_loadgen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF38E7E-B781-6047-8298-7D6A26799A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0490CABA-3A31-684A-9C02-C447D78D22AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1300" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{5A3F0FCA-A9DB-A84C-AEE3-F88E9CDDE907}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="87">
   <si>
     <t>name</t>
   </si>
@@ -79,9 +79,6 @@
     <t>current_source</t>
   </si>
   <si>
-    <t>PV</t>
-  </si>
-  <si>
     <t>vm_pu</t>
   </si>
   <si>
@@ -302,6 +299,12 @@
   </si>
   <si>
     <t>63/25/38 MVA 110/20/10 kV</t>
+  </si>
+  <si>
+    <t>pv</t>
+  </si>
+  <si>
+    <t>PV-gen</t>
   </si>
 </sst>
 </file>
@@ -816,7 +819,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F413700-575B-114F-8714-9F90937FF260}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="A2:J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -850,36 +855,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1.2E-2</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -888,10 +864,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476D1716-E415-9148-A59A-7D3D790AE6BA}">
-  <dimension ref="B1:N1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -900,7 +876,7 @@
     <col min="14" max="14" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -911,34 +887,69 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>1.03</v>
+      </c>
+      <c r="G2">
+        <v>-3</v>
+      </c>
+      <c r="H2">
+        <v>-3</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -962,13 +973,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>8</v>
@@ -1012,67 +1023,67 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>8</v>
@@ -1083,10 +1094,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1119,7 +1130,7 @@
         <v>150</v>
       </c>
       <c r="N2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -1168,112 +1179,112 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD1" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="AE1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="AF1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="AL1" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1307,13 +1318,13 @@
         <v>6</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>7</v>
@@ -1343,57 +1354,57 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2">
         <v>0.06</v>
@@ -1420,10 +1431,10 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1446,7 +1457,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3">
         <v>0.06</v>
@@ -1473,10 +1484,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1499,7 +1510,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4">
         <v>0.04</v>
@@ -1526,10 +1537,10 @@
         <v>150</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1552,7 +1563,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>0.05</v>
@@ -1579,10 +1590,10 @@
         <v>150</v>
       </c>
       <c r="J5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -1605,7 +1616,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6">
         <v>7.0000000000000007E-2</v>
@@ -1632,10 +1643,10 @@
         <v>150</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -1658,7 +1669,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7">
         <v>0.04</v>
@@ -1685,10 +1696,10 @@
         <v>150</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1711,7 +1722,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8">
         <v>0.05</v>
@@ -1738,10 +1749,10 @@
         <v>150</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1764,7 +1775,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9">
         <v>7.0000000000000007E-2</v>
@@ -1791,10 +1802,10 @@
         <v>150</v>
       </c>
       <c r="J9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1817,7 +1828,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10">
         <v>0.32</v>
@@ -1844,10 +1855,10 @@
         <v>150</v>
       </c>
       <c r="J10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1870,7 +1881,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11">
         <v>0.33750000000000002</v>
@@ -1897,10 +1908,10 @@
         <v>150</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1923,7 +1934,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12">
         <v>0.26190000000000002</v>
@@ -1950,10 +1961,10 @@
         <v>150</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1976,7 +1987,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13">
         <v>0.24</v>
@@ -2003,10 +2014,10 @@
         <v>150</v>
       </c>
       <c r="J13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -2029,7 +2040,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14">
         <v>0.23749999999999999</v>
@@ -2056,10 +2067,10 @@
         <v>150</v>
       </c>
       <c r="J14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -2082,7 +2093,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>0.18729999999999999</v>
@@ -2109,10 +2120,10 @@
         <v>150</v>
       </c>
       <c r="J15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -2150,75 +2161,75 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>63</v>
@@ -2269,10 +2280,10 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T2">
         <v>0</v>
@@ -2289,7 +2300,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <v>63</v>
@@ -2340,10 +2351,10 @@
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T3">
         <v>0</v>

</xml_diff>